<commit_message>
Cleaned up formatting for 2018
Add player name & injury type
</commit_message>
<xml_diff>
--- a/2020_NCAAF_Injuries.xlsx
+++ b/2020_NCAAF_Injuries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aditirajagopal/Documents/repos/ncaa_football_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24D4A56-65E3-2B44-872A-9D2A87134583}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA4F70C-53EF-4847-B3CA-0224C8428155}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{92438842-A20E-7849-BBB4-16B462A4BE03}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="8760" xr2:uid="{92438842-A20E-7849-BBB4-16B462A4BE03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -2778,7 +2778,7 @@
   <dimension ref="A1:F715"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F1" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -14072,74 +14072,74 @@
     <hyperlink ref="A231" r:id="rId40" display="http://statfox.com/cfb/cfbteam.asp?teamid=LA+LAFAYETTE" xr:uid="{D2D5BD72-5BBC-424B-B522-A3ABB0DE2AB1}"/>
     <hyperlink ref="A238" r:id="rId41" display="http://statfox.com/cfb/cfbteam.asp?teamid=LA+MONROE" xr:uid="{F16D7EEB-7ABC-E948-B0ED-4F06755BC29B}"/>
     <hyperlink ref="A240" r:id="rId42" display="http://statfox.com/cfb/cfbteam.asp?teamid=LOUISIANA+TECH" xr:uid="{DC06F82B-4855-9B49-8A5B-FDE9DEBA97C5}"/>
-    <hyperlink ref="A243" r:id="rId43" display="http://statfox.com/cfb/cfbteam.asp?teamid=LOUISVILLE" xr:uid="{533BBDB9-CAC5-494E-ACF2-9FEE5595F7AE}"/>
-    <hyperlink ref="A246" r:id="rId44" display="http://statfox.com/cfb/cfbteam.asp?teamid=LSU" xr:uid="{64CD9178-7FE8-EE45-81F6-21B38FA7AF7A}"/>
-    <hyperlink ref="A254" r:id="rId45" display="http://statfox.com/cfb/cfbteam.asp?teamid=MARSHALL" xr:uid="{E148567F-7C52-B445-8EA2-752593457042}"/>
-    <hyperlink ref="A263" r:id="rId46" display="http://statfox.com/cfb/cfbteam.asp?teamid=MARYLAND" xr:uid="{BF04D3BD-E226-3143-AFED-2ACE365F5B6E}"/>
-    <hyperlink ref="A265" r:id="rId47" display="http://statfox.com/cfb/cfbteam.asp?teamid=MASSACHUSETTS" xr:uid="{7DB2A592-3763-8B4B-B9D7-63CADECCBBFB}"/>
-    <hyperlink ref="A269" r:id="rId48" display="http://statfox.com/cfb/cfbteam.asp?teamid=MEMPHIS" xr:uid="{1C173C5A-AD96-1441-A05C-D5708111EA5A}"/>
-    <hyperlink ref="A278" r:id="rId49" display="http://statfox.com/cfb/cfbteam.asp?teamid=MIAMI" xr:uid="{436FE9E1-A3AA-944B-A5ED-D067A0ACF3D8}"/>
-    <hyperlink ref="A291" r:id="rId50" display="http://statfox.com/cfb/cfbteam.asp?teamid=MICHIGAN" xr:uid="{7C8742EC-566C-F34E-A78E-5F19EEF84F7B}"/>
-    <hyperlink ref="A297" r:id="rId51" display="http://statfox.com/cfb/cfbteam.asp?teamid=MICHIGAN+ST" xr:uid="{A2B19D59-E249-B64F-ADA9-BED02BF92A1A}"/>
-    <hyperlink ref="A303" r:id="rId52" display="http://statfox.com/cfb/cfbteam.asp?teamid=MIDDLE+TENN+ST" xr:uid="{9E9FA7D2-713C-7343-80EE-CCEB13D7B26B}"/>
-    <hyperlink ref="A308" r:id="rId53" display="http://statfox.com/cfb/cfbteam.asp?teamid=MINNESOTA" xr:uid="{29D55647-3E86-9F40-8B85-481A177C3E86}"/>
-    <hyperlink ref="A316" r:id="rId54" display="http://statfox.com/cfb/cfbteam.asp?teamid=MISSISSIPPI+ST" xr:uid="{A83FDC3C-315D-0C4F-9834-8AC28D099D3D}"/>
-    <hyperlink ref="A321" r:id="rId55" display="http://statfox.com/cfb/cfbteam.asp?teamid=MISSOURI" xr:uid="{7338116B-0672-2747-88D1-30D873C653AD}"/>
-    <hyperlink ref="A335" r:id="rId56" display="http://statfox.com/cfb/cfbteam.asp?teamid=N+CAROLINA" xr:uid="{793D781A-E469-7C42-ADEA-F8D855FF963D}"/>
-    <hyperlink ref="A346" r:id="rId57" display="http://statfox.com/cfb/cfbteam.asp?teamid=N+ILLINOIS" xr:uid="{F7F3802D-A5F3-374F-8DBA-3A74BC3DBCF3}"/>
-    <hyperlink ref="A349" r:id="rId58" display="http://statfox.com/cfb/cfbteam.asp?teamid=NAVY" xr:uid="{650C5BAB-427A-464F-8874-FCE6633AA827}"/>
-    <hyperlink ref="A354" r:id="rId59" display="http://statfox.com/cfb/cfbteam.asp?teamid=NC+STATE" xr:uid="{AB56BC01-E447-AF45-99D0-403BD197A98B}"/>
-    <hyperlink ref="A364" r:id="rId60" display="http://statfox.com/cfb/cfbteam.asp?teamid=NEBRASKA" xr:uid="{E56A1039-DA7C-9F4A-9008-A85067A7E90E}"/>
-    <hyperlink ref="A372" r:id="rId61" display="http://statfox.com/cfb/cfbteam.asp?teamid=NEVADA" xr:uid="{121044DC-ACE8-8B45-A312-52ADC194AC0C}"/>
-    <hyperlink ref="A380" r:id="rId62" display="http://statfox.com/cfb/cfbteam.asp?teamid=NORTH+TEXAS" xr:uid="{855A9440-14F2-4344-A61E-4385BF77B4CB}"/>
-    <hyperlink ref="A386" r:id="rId63" display="http://statfox.com/cfb/cfbteam.asp?teamid=NORTHWESTERN" xr:uid="{5747E0E5-CB87-BA42-876B-45EA4A9C3549}"/>
-    <hyperlink ref="A394" r:id="rId64" display="http://statfox.com/cfb/cfbteam.asp?teamid=NOTRE+DAME" xr:uid="{8952CA6A-FB70-A14F-8000-B757D0C26A31}"/>
-    <hyperlink ref="A401" r:id="rId65" display="http://statfox.com/cfb/cfbteam.asp?teamid=OHIO+ST" xr:uid="{1EF48968-D8F9-044B-B930-4DC974B715E9}"/>
-    <hyperlink ref="A417" r:id="rId66" display="http://statfox.com/cfb/cfbteam.asp?teamid=OKLAHOMA" xr:uid="{BEFEBA03-A61A-5342-AA0F-8A660CE6009A}"/>
-    <hyperlink ref="A432" r:id="rId67" display="http://statfox.com/cfb/cfbteam.asp?teamid=OKLAHOMA+ST" xr:uid="{D5618D0C-A34D-6141-A139-8EA47493CD79}"/>
-    <hyperlink ref="A436" r:id="rId68" display="http://statfox.com/cfb/cfbteam.asp?teamid=OLD+DOMINION" xr:uid="{F0113423-AACC-9A4A-A2CB-39FD759A94EB}"/>
-    <hyperlink ref="A438" r:id="rId69" display="http://statfox.com/cfb/cfbteam.asp?teamid=OLE+MISS" xr:uid="{B509A1E0-6FA9-1D4E-80D1-353B4CFABE01}"/>
-    <hyperlink ref="A441" r:id="rId70" display="http://statfox.com/cfb/cfbteam.asp?teamid=OREGON" xr:uid="{FB3B89F7-72F3-3940-A84F-2434BB8B5EB5}"/>
-    <hyperlink ref="A448" r:id="rId71" display="http://statfox.com/cfb/cfbteam.asp?teamid=OREGON+ST" xr:uid="{F604CE52-B396-1E44-BE8B-83C7D251ED7E}"/>
-    <hyperlink ref="A450" r:id="rId72" display="http://statfox.com/cfb/cfbteam.asp?teamid=PENN+ST" xr:uid="{A0D98464-D7F0-BC4B-BD0B-416BB8C39230}"/>
-    <hyperlink ref="A456" r:id="rId73" display="http://statfox.com/cfb/cfbteam.asp?teamid=PITTSBURGH" xr:uid="{D938809F-E2B9-7846-B955-513A473F2285}"/>
-    <hyperlink ref="A467" r:id="rId74" display="http://statfox.com/cfb/cfbteam.asp?teamid=PURDUE" xr:uid="{D776D27A-00EF-524F-B849-BEEE92E62FAE}"/>
-    <hyperlink ref="A474" r:id="rId75" display="http://statfox.com/cfb/cfbteam.asp?teamid=RICE" xr:uid="{D030DABD-90F1-3A40-8D60-4838F52204AB}"/>
-    <hyperlink ref="A476" r:id="rId76" display="http://statfox.com/cfb/cfbteam.asp?teamid=S+ALABAMA" xr:uid="{46A37EC1-EFDD-C640-A9CE-61D09EF7A548}"/>
-    <hyperlink ref="A478" r:id="rId77" display="http://statfox.com/cfb/cfbteam.asp?teamid=S+CAROLINA" xr:uid="{13DB7133-4F38-DA47-A457-589B20B082EA}"/>
-    <hyperlink ref="A488" r:id="rId78" display="http://statfox.com/cfb/cfbteam.asp?teamid=S+FLORIDA" xr:uid="{CB16F385-621E-9F41-BCFE-A7EBD262E22A}"/>
-    <hyperlink ref="A502" r:id="rId79" display="http://statfox.com/cfb/cfbteam.asp?teamid=SMU" xr:uid="{5FBB5242-D94C-7F48-B88B-70E0EDD2A5EA}"/>
-    <hyperlink ref="A507" r:id="rId80" display="http://statfox.com/cfb/cfbteam.asp?teamid=SOUTHERN+MISS" xr:uid="{EC1AEB50-FE82-0F4B-9F58-01BC862FDCA8}"/>
-    <hyperlink ref="A512" r:id="rId81" display="http://statfox.com/cfb/cfbteam.asp?teamid=STANFORD" xr:uid="{B0C4D55F-F65A-F344-A623-4164F7D29461}"/>
-    <hyperlink ref="A516" r:id="rId82" display="http://statfox.com/cfb/cfbteam.asp?teamid=SYRACUSE" xr:uid="{0346771B-2BE9-6E47-B993-CA797504561A}"/>
-    <hyperlink ref="A534" r:id="rId83" display="http://statfox.com/cfb/cfbteam.asp?teamid=TCU" xr:uid="{97B2126D-76AF-054F-AC45-FBE2E22E586A}"/>
-    <hyperlink ref="A543" r:id="rId84" display="http://statfox.com/cfb/cfbteam.asp?teamid=TEMPLE" xr:uid="{7139927D-4641-D440-8E57-578999489881}"/>
-    <hyperlink ref="A553" r:id="rId85" display="http://statfox.com/cfb/cfbteam.asp?teamid=TENNESSEE" xr:uid="{3ECB2DA1-41F9-7E48-BC8D-D1C49C26A3DD}"/>
-    <hyperlink ref="A559" r:id="rId86" display="http://statfox.com/cfb/cfbteam.asp?teamid=TEXAS" xr:uid="{C4C9BB23-DAA2-654E-84A8-F42FB296824A}"/>
-    <hyperlink ref="A573" r:id="rId87" display="http://statfox.com/cfb/cfbteam.asp?teamid=TEXAS+A%26M" xr:uid="{BC8DD9F0-B98A-F14D-BF37-D24C50B369ED}"/>
-    <hyperlink ref="A584" r:id="rId88" display="http://statfox.com/cfb/cfbteam.asp?teamid=TEXAS+ST" xr:uid="{9B3787CC-F29F-EA41-B428-EA8580DF4584}"/>
-    <hyperlink ref="A589" r:id="rId89" display="http://statfox.com/cfb/cfbteam.asp?teamid=TEXAS+TECH" xr:uid="{6F1D0596-8B30-7345-9460-F41FC84C291C}"/>
-    <hyperlink ref="A605" r:id="rId90" display="http://statfox.com/cfb/cfbteam.asp?teamid=TROY" xr:uid="{BF4C38E1-CF28-024F-B690-452D11F9428E}"/>
-    <hyperlink ref="A607" r:id="rId91" display="http://statfox.com/cfb/cfbteam.asp?teamid=TULANE" xr:uid="{C01D48D6-A709-CF44-AA3A-D40316D3D21B}"/>
-    <hyperlink ref="A611" r:id="rId92" display="http://statfox.com/cfb/cfbteam.asp?teamid=TULSA" xr:uid="{A4C0F558-226C-484C-A692-6C302993AD72}"/>
-    <hyperlink ref="A616" r:id="rId93" display="http://statfox.com/cfb/cfbteam.asp?teamid=UAB" xr:uid="{D5776D7E-D699-0C47-B6C3-8ED52879F035}"/>
-    <hyperlink ref="A618" r:id="rId94" display="http://statfox.com/cfb/cfbteam.asp?teamid=UCF" xr:uid="{D463CD41-E360-DB4C-87F1-18082E336255}"/>
-    <hyperlink ref="A633" r:id="rId95" display="http://statfox.com/cfb/cfbteam.asp?teamid=UCLA" xr:uid="{89E9BAA5-BCF6-1B45-847B-1223FE6B8DA8}"/>
-    <hyperlink ref="A638" r:id="rId96" display="http://statfox.com/cfb/cfbteam.asp?teamid=UNLV" xr:uid="{F9FDF600-16F1-D344-9DE1-B60572144B69}"/>
-    <hyperlink ref="A640" r:id="rId97" display="http://statfox.com/cfb/cfbteam.asp?teamid=USC" xr:uid="{2D4673F3-BF90-2348-9A82-450800B122AE}"/>
-    <hyperlink ref="A645" r:id="rId98" display="http://statfox.com/cfb/cfbteam.asp?teamid=UTAH" xr:uid="{EB55A55A-01B0-6943-A1DF-C814815C8A00}"/>
-    <hyperlink ref="A648" r:id="rId99" display="http://statfox.com/cfb/cfbteam.asp?teamid=UTEP" xr:uid="{5B89B8DD-CFA2-9541-B519-E92ED3A9E2DC}"/>
-    <hyperlink ref="A650" r:id="rId100" display="http://statfox.com/cfb/cfbteam.asp?teamid=VANDERBILT" xr:uid="{FA2C59AE-56E3-AD4A-96F0-15864D228B80}"/>
-    <hyperlink ref="A663" r:id="rId101" display="http://statfox.com/cfb/cfbteam.asp?teamid=VIRGINIA" xr:uid="{948182C3-3F5A-8D47-8A52-F0FFDC30B10D}"/>
-    <hyperlink ref="A668" r:id="rId102" display="http://statfox.com/cfb/cfbteam.asp?teamid=VIRGINIA+TECH" xr:uid="{B7B941D2-7DB0-DE47-8D92-DC5BC98574D9}"/>
-    <hyperlink ref="A678" r:id="rId103" display="http://statfox.com/cfb/cfbteam.asp?teamid=W+KENTUCKY" xr:uid="{EA17F1BE-E2F6-2741-979F-3F29C26E064A}"/>
-    <hyperlink ref="A680" r:id="rId104" display="http://statfox.com/cfb/cfbteam.asp?teamid=W+MICHIGAN" xr:uid="{5B17644F-2C36-4547-A45C-1C532734F966}"/>
-    <hyperlink ref="A683" r:id="rId105" display="http://statfox.com/cfb/cfbteam.asp?teamid=W+VIRGINIA" xr:uid="{80901308-9DD4-E44B-AEC2-6AEE88E771B4}"/>
-    <hyperlink ref="A690" r:id="rId106" display="http://statfox.com/cfb/cfbteam.asp?teamid=WAKE+FOREST" xr:uid="{94DE4B0A-9C4C-8949-AF54-2153B699F33E}"/>
-    <hyperlink ref="A696" r:id="rId107" display="http://statfox.com/cfb/cfbteam.asp?teamid=WASHINGTON" xr:uid="{A8049B1A-E4BE-B844-B79C-4CD4F5A5F7AA}"/>
-    <hyperlink ref="A700" r:id="rId108" display="http://statfox.com/cfb/cfbteam.asp?teamid=WASHINGTON+ST" xr:uid="{9151FDDF-56AE-3D41-B85E-2BADB23DDFF5}"/>
-    <hyperlink ref="A702" r:id="rId109" display="http://statfox.com/cfb/cfbteam.asp?teamid=WISCONSIN" xr:uid="{C428BC65-B7D3-0741-BBEE-DC6DB2A4968C}"/>
-    <hyperlink ref="A710" r:id="rId110" display="http://statfox.com/cfb/cfbteam.asp?teamid=WYOMING" xr:uid="{3142122C-5F98-434F-A16B-6D32F681749B}"/>
+    <hyperlink ref="A246" r:id="rId43" display="http://statfox.com/cfb/cfbteam.asp?teamid=LSU" xr:uid="{64CD9178-7FE8-EE45-81F6-21B38FA7AF7A}"/>
+    <hyperlink ref="A254" r:id="rId44" display="http://statfox.com/cfb/cfbteam.asp?teamid=MARSHALL" xr:uid="{E148567F-7C52-B445-8EA2-752593457042}"/>
+    <hyperlink ref="A263" r:id="rId45" display="http://statfox.com/cfb/cfbteam.asp?teamid=MARYLAND" xr:uid="{BF04D3BD-E226-3143-AFED-2ACE365F5B6E}"/>
+    <hyperlink ref="A265" r:id="rId46" display="http://statfox.com/cfb/cfbteam.asp?teamid=MASSACHUSETTS" xr:uid="{7DB2A592-3763-8B4B-B9D7-63CADECCBBFB}"/>
+    <hyperlink ref="A269" r:id="rId47" display="http://statfox.com/cfb/cfbteam.asp?teamid=MEMPHIS" xr:uid="{1C173C5A-AD96-1441-A05C-D5708111EA5A}"/>
+    <hyperlink ref="A278" r:id="rId48" display="http://statfox.com/cfb/cfbteam.asp?teamid=MIAMI" xr:uid="{436FE9E1-A3AA-944B-A5ED-D067A0ACF3D8}"/>
+    <hyperlink ref="A291" r:id="rId49" display="http://statfox.com/cfb/cfbteam.asp?teamid=MICHIGAN" xr:uid="{7C8742EC-566C-F34E-A78E-5F19EEF84F7B}"/>
+    <hyperlink ref="A297" r:id="rId50" display="http://statfox.com/cfb/cfbteam.asp?teamid=MICHIGAN+ST" xr:uid="{A2B19D59-E249-B64F-ADA9-BED02BF92A1A}"/>
+    <hyperlink ref="A303" r:id="rId51" display="http://statfox.com/cfb/cfbteam.asp?teamid=MIDDLE+TENN+ST" xr:uid="{9E9FA7D2-713C-7343-80EE-CCEB13D7B26B}"/>
+    <hyperlink ref="A308" r:id="rId52" display="http://statfox.com/cfb/cfbteam.asp?teamid=MINNESOTA" xr:uid="{29D55647-3E86-9F40-8B85-481A177C3E86}"/>
+    <hyperlink ref="A316" r:id="rId53" display="http://statfox.com/cfb/cfbteam.asp?teamid=MISSISSIPPI+ST" xr:uid="{A83FDC3C-315D-0C4F-9834-8AC28D099D3D}"/>
+    <hyperlink ref="A321" r:id="rId54" display="http://statfox.com/cfb/cfbteam.asp?teamid=MISSOURI" xr:uid="{7338116B-0672-2747-88D1-30D873C653AD}"/>
+    <hyperlink ref="A335" r:id="rId55" display="http://statfox.com/cfb/cfbteam.asp?teamid=N+CAROLINA" xr:uid="{793D781A-E469-7C42-ADEA-F8D855FF963D}"/>
+    <hyperlink ref="A346" r:id="rId56" display="http://statfox.com/cfb/cfbteam.asp?teamid=N+ILLINOIS" xr:uid="{F7F3802D-A5F3-374F-8DBA-3A74BC3DBCF3}"/>
+    <hyperlink ref="A349" r:id="rId57" display="http://statfox.com/cfb/cfbteam.asp?teamid=NAVY" xr:uid="{650C5BAB-427A-464F-8874-FCE6633AA827}"/>
+    <hyperlink ref="A354" r:id="rId58" display="http://statfox.com/cfb/cfbteam.asp?teamid=NC+STATE" xr:uid="{AB56BC01-E447-AF45-99D0-403BD197A98B}"/>
+    <hyperlink ref="A364" r:id="rId59" display="http://statfox.com/cfb/cfbteam.asp?teamid=NEBRASKA" xr:uid="{E56A1039-DA7C-9F4A-9008-A85067A7E90E}"/>
+    <hyperlink ref="A372" r:id="rId60" display="http://statfox.com/cfb/cfbteam.asp?teamid=NEVADA" xr:uid="{121044DC-ACE8-8B45-A312-52ADC194AC0C}"/>
+    <hyperlink ref="A380" r:id="rId61" display="http://statfox.com/cfb/cfbteam.asp?teamid=NORTH+TEXAS" xr:uid="{855A9440-14F2-4344-A61E-4385BF77B4CB}"/>
+    <hyperlink ref="A386" r:id="rId62" display="http://statfox.com/cfb/cfbteam.asp?teamid=NORTHWESTERN" xr:uid="{5747E0E5-CB87-BA42-876B-45EA4A9C3549}"/>
+    <hyperlink ref="A394" r:id="rId63" display="http://statfox.com/cfb/cfbteam.asp?teamid=NOTRE+DAME" xr:uid="{8952CA6A-FB70-A14F-8000-B757D0C26A31}"/>
+    <hyperlink ref="A401" r:id="rId64" display="http://statfox.com/cfb/cfbteam.asp?teamid=OHIO+ST" xr:uid="{1EF48968-D8F9-044B-B930-4DC974B715E9}"/>
+    <hyperlink ref="A417" r:id="rId65" display="http://statfox.com/cfb/cfbteam.asp?teamid=OKLAHOMA" xr:uid="{BEFEBA03-A61A-5342-AA0F-8A660CE6009A}"/>
+    <hyperlink ref="A432" r:id="rId66" display="http://statfox.com/cfb/cfbteam.asp?teamid=OKLAHOMA+ST" xr:uid="{D5618D0C-A34D-6141-A139-8EA47493CD79}"/>
+    <hyperlink ref="A436" r:id="rId67" display="http://statfox.com/cfb/cfbteam.asp?teamid=OLD+DOMINION" xr:uid="{F0113423-AACC-9A4A-A2CB-39FD759A94EB}"/>
+    <hyperlink ref="A438" r:id="rId68" display="http://statfox.com/cfb/cfbteam.asp?teamid=OLE+MISS" xr:uid="{B509A1E0-6FA9-1D4E-80D1-353B4CFABE01}"/>
+    <hyperlink ref="A441" r:id="rId69" display="http://statfox.com/cfb/cfbteam.asp?teamid=OREGON" xr:uid="{FB3B89F7-72F3-3940-A84F-2434BB8B5EB5}"/>
+    <hyperlink ref="A448" r:id="rId70" display="http://statfox.com/cfb/cfbteam.asp?teamid=OREGON+ST" xr:uid="{F604CE52-B396-1E44-BE8B-83C7D251ED7E}"/>
+    <hyperlink ref="A450" r:id="rId71" display="http://statfox.com/cfb/cfbteam.asp?teamid=PENN+ST" xr:uid="{A0D98464-D7F0-BC4B-BD0B-416BB8C39230}"/>
+    <hyperlink ref="A456" r:id="rId72" display="http://statfox.com/cfb/cfbteam.asp?teamid=PITTSBURGH" xr:uid="{D938809F-E2B9-7846-B955-513A473F2285}"/>
+    <hyperlink ref="A467" r:id="rId73" display="http://statfox.com/cfb/cfbteam.asp?teamid=PURDUE" xr:uid="{D776D27A-00EF-524F-B849-BEEE92E62FAE}"/>
+    <hyperlink ref="A474" r:id="rId74" display="http://statfox.com/cfb/cfbteam.asp?teamid=RICE" xr:uid="{D030DABD-90F1-3A40-8D60-4838F52204AB}"/>
+    <hyperlink ref="A476" r:id="rId75" display="http://statfox.com/cfb/cfbteam.asp?teamid=S+ALABAMA" xr:uid="{46A37EC1-EFDD-C640-A9CE-61D09EF7A548}"/>
+    <hyperlink ref="A478" r:id="rId76" display="http://statfox.com/cfb/cfbteam.asp?teamid=S+CAROLINA" xr:uid="{13DB7133-4F38-DA47-A457-589B20B082EA}"/>
+    <hyperlink ref="A488" r:id="rId77" display="http://statfox.com/cfb/cfbteam.asp?teamid=S+FLORIDA" xr:uid="{CB16F385-621E-9F41-BCFE-A7EBD262E22A}"/>
+    <hyperlink ref="A502" r:id="rId78" display="http://statfox.com/cfb/cfbteam.asp?teamid=SMU" xr:uid="{5FBB5242-D94C-7F48-B88B-70E0EDD2A5EA}"/>
+    <hyperlink ref="A507" r:id="rId79" display="http://statfox.com/cfb/cfbteam.asp?teamid=SOUTHERN+MISS" xr:uid="{EC1AEB50-FE82-0F4B-9F58-01BC862FDCA8}"/>
+    <hyperlink ref="A512" r:id="rId80" display="http://statfox.com/cfb/cfbteam.asp?teamid=STANFORD" xr:uid="{B0C4D55F-F65A-F344-A623-4164F7D29461}"/>
+    <hyperlink ref="A516" r:id="rId81" display="http://statfox.com/cfb/cfbteam.asp?teamid=SYRACUSE" xr:uid="{0346771B-2BE9-6E47-B993-CA797504561A}"/>
+    <hyperlink ref="A534" r:id="rId82" display="http://statfox.com/cfb/cfbteam.asp?teamid=TCU" xr:uid="{97B2126D-76AF-054F-AC45-FBE2E22E586A}"/>
+    <hyperlink ref="A543" r:id="rId83" display="http://statfox.com/cfb/cfbteam.asp?teamid=TEMPLE" xr:uid="{7139927D-4641-D440-8E57-578999489881}"/>
+    <hyperlink ref="A553" r:id="rId84" display="http://statfox.com/cfb/cfbteam.asp?teamid=TENNESSEE" xr:uid="{3ECB2DA1-41F9-7E48-BC8D-D1C49C26A3DD}"/>
+    <hyperlink ref="A559" r:id="rId85" display="http://statfox.com/cfb/cfbteam.asp?teamid=TEXAS" xr:uid="{C4C9BB23-DAA2-654E-84A8-F42FB296824A}"/>
+    <hyperlink ref="A573" r:id="rId86" display="http://statfox.com/cfb/cfbteam.asp?teamid=TEXAS+A%26M" xr:uid="{BC8DD9F0-B98A-F14D-BF37-D24C50B369ED}"/>
+    <hyperlink ref="A584" r:id="rId87" display="http://statfox.com/cfb/cfbteam.asp?teamid=TEXAS+ST" xr:uid="{9B3787CC-F29F-EA41-B428-EA8580DF4584}"/>
+    <hyperlink ref="A589" r:id="rId88" display="http://statfox.com/cfb/cfbteam.asp?teamid=TEXAS+TECH" xr:uid="{6F1D0596-8B30-7345-9460-F41FC84C291C}"/>
+    <hyperlink ref="A605" r:id="rId89" display="http://statfox.com/cfb/cfbteam.asp?teamid=TROY" xr:uid="{BF4C38E1-CF28-024F-B690-452D11F9428E}"/>
+    <hyperlink ref="A607" r:id="rId90" display="http://statfox.com/cfb/cfbteam.asp?teamid=TULANE" xr:uid="{C01D48D6-A709-CF44-AA3A-D40316D3D21B}"/>
+    <hyperlink ref="A611" r:id="rId91" display="http://statfox.com/cfb/cfbteam.asp?teamid=TULSA" xr:uid="{A4C0F558-226C-484C-A692-6C302993AD72}"/>
+    <hyperlink ref="A616" r:id="rId92" display="http://statfox.com/cfb/cfbteam.asp?teamid=UAB" xr:uid="{D5776D7E-D699-0C47-B6C3-8ED52879F035}"/>
+    <hyperlink ref="A618" r:id="rId93" display="http://statfox.com/cfb/cfbteam.asp?teamid=UCF" xr:uid="{D463CD41-E360-DB4C-87F1-18082E336255}"/>
+    <hyperlink ref="A633" r:id="rId94" display="http://statfox.com/cfb/cfbteam.asp?teamid=UCLA" xr:uid="{89E9BAA5-BCF6-1B45-847B-1223FE6B8DA8}"/>
+    <hyperlink ref="A638" r:id="rId95" display="http://statfox.com/cfb/cfbteam.asp?teamid=UNLV" xr:uid="{F9FDF600-16F1-D344-9DE1-B60572144B69}"/>
+    <hyperlink ref="A640" r:id="rId96" display="http://statfox.com/cfb/cfbteam.asp?teamid=USC" xr:uid="{2D4673F3-BF90-2348-9A82-450800B122AE}"/>
+    <hyperlink ref="A645" r:id="rId97" display="http://statfox.com/cfb/cfbteam.asp?teamid=UTAH" xr:uid="{EB55A55A-01B0-6943-A1DF-C814815C8A00}"/>
+    <hyperlink ref="A648" r:id="rId98" display="http://statfox.com/cfb/cfbteam.asp?teamid=UTEP" xr:uid="{5B89B8DD-CFA2-9541-B519-E92ED3A9E2DC}"/>
+    <hyperlink ref="A650" r:id="rId99" display="http://statfox.com/cfb/cfbteam.asp?teamid=VANDERBILT" xr:uid="{FA2C59AE-56E3-AD4A-96F0-15864D228B80}"/>
+    <hyperlink ref="A663" r:id="rId100" display="http://statfox.com/cfb/cfbteam.asp?teamid=VIRGINIA" xr:uid="{948182C3-3F5A-8D47-8A52-F0FFDC30B10D}"/>
+    <hyperlink ref="A668" r:id="rId101" display="http://statfox.com/cfb/cfbteam.asp?teamid=VIRGINIA+TECH" xr:uid="{B7B941D2-7DB0-DE47-8D92-DC5BC98574D9}"/>
+    <hyperlink ref="A678" r:id="rId102" display="http://statfox.com/cfb/cfbteam.asp?teamid=W+KENTUCKY" xr:uid="{EA17F1BE-E2F6-2741-979F-3F29C26E064A}"/>
+    <hyperlink ref="A680" r:id="rId103" display="http://statfox.com/cfb/cfbteam.asp?teamid=W+MICHIGAN" xr:uid="{5B17644F-2C36-4547-A45C-1C532734F966}"/>
+    <hyperlink ref="A683" r:id="rId104" display="http://statfox.com/cfb/cfbteam.asp?teamid=W+VIRGINIA" xr:uid="{80901308-9DD4-E44B-AEC2-6AEE88E771B4}"/>
+    <hyperlink ref="A690" r:id="rId105" display="http://statfox.com/cfb/cfbteam.asp?teamid=WAKE+FOREST" xr:uid="{94DE4B0A-9C4C-8949-AF54-2153B699F33E}"/>
+    <hyperlink ref="A696" r:id="rId106" display="http://statfox.com/cfb/cfbteam.asp?teamid=WASHINGTON" xr:uid="{A8049B1A-E4BE-B844-B79C-4CD4F5A5F7AA}"/>
+    <hyperlink ref="A700" r:id="rId107" display="http://statfox.com/cfb/cfbteam.asp?teamid=WASHINGTON+ST" xr:uid="{9151FDDF-56AE-3D41-B85E-2BADB23DDFF5}"/>
+    <hyperlink ref="A702" r:id="rId108" display="http://statfox.com/cfb/cfbteam.asp?teamid=WISCONSIN" xr:uid="{C428BC65-B7D3-0741-BBEE-DC6DB2A4968C}"/>
+    <hyperlink ref="A710" r:id="rId109" display="http://statfox.com/cfb/cfbteam.asp?teamid=WYOMING" xr:uid="{3142122C-5F98-434F-A16B-6D32F681749B}"/>
+    <hyperlink ref="A243" r:id="rId110" display="http://statfox.com/cfb/cfbteam.asp?teamid=LOUISVILLE" xr:uid="{533BBDB9-CAC5-494E-ACF2-9FEE5595F7AE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>